<commit_message>
apresentação e ajuste documentos
</commit_message>
<xml_diff>
--- a/SCRUM_apoio.xlsx
+++ b/SCRUM_apoio.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dados\01-Votorantim\01-VPAR\00-Novas Tecnologias\2022\99-TEX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B62EA1-616E-4C02-B242-11BC3A3D4F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7282B6-32C5-4AFD-BD18-3DB03A4B697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories" sheetId="1" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="4" r:id="rId2"/>
     <sheet name="Sprint Planning" sheetId="5" r:id="rId3"/>
-    <sheet name="UserStoryPoints" sheetId="3" r:id="rId4"/>
-    <sheet name="BurnDown" sheetId="2" r:id="rId5"/>
+    <sheet name="Valor Estimado" sheetId="6" r:id="rId4"/>
+    <sheet name="UserStoryPoints" sheetId="3" r:id="rId5"/>
+    <sheet name="BurnDown" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="nome_projeto">'Product Backlog'!$B$4</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="300">
   <si>
     <t>Gráfico BurnDown - Exemplo</t>
   </si>
@@ -1643,9 +1644,6 @@
     <t>Features x Sprints</t>
   </si>
   <si>
-    <t>Sprint Planning</t>
-  </si>
-  <si>
     <r>
       <t>Feature 01</t>
     </r>
@@ -1828,9 +1826,6 @@
     <t>Story # 7</t>
   </si>
   <si>
-    <t>Func. Persona 02 - Conectada</t>
-  </si>
-  <si>
     <t>Story # 8</t>
   </si>
   <si>
@@ -1895,13 +1890,273 @@
   </si>
   <si>
     <t>Iniciamente implementar um bot de atendimento que possa ir sendo melhorado com o tempo, incorporando as novas dúvidas e mesmo soluções. Além do bot podemos orçar uma equipe humana (mnima´) que possa atender também via whatsapp em modelo de callback (deverá ter SLA adequado). E uma alternativa para manuais serão videos curtos sobre as principais dúvidas, usando avatares ou personagens fictícios para exemplificar o problema e/ou solução - lembrando que precisam ser curtos, no máximo 01 minuto - mais do que isso o risco é perder o cliente.</t>
+  </si>
+  <si>
+    <t>Falta</t>
+  </si>
+  <si>
+    <t>Dividir equipe até amanhã a noite, para se prepararem para quinta!</t>
+  </si>
+  <si>
+    <t>Quem vai apresentar? Sequencia!</t>
+  </si>
+  <si>
+    <t>70 - Para motivar usuários da "Melhor idade"</t>
+  </si>
+  <si>
+    <t>Gabriel Verissimo</t>
+  </si>
+  <si>
+    <t>Gabriel Guilherme</t>
+  </si>
+  <si>
+    <t>Gabriel Ramalho</t>
+  </si>
+  <si>
+    <t>Felipe Souza</t>
+  </si>
+  <si>
+    <t>Diego Trindade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernando </t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>Comex</t>
+  </si>
+  <si>
+    <t>TiozaoRH</t>
+  </si>
+  <si>
+    <t>Antenada</t>
+  </si>
+  <si>
+    <t>Gestão Projeto e Citação</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>b, c</t>
+  </si>
+  <si>
+    <t>d, f</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Tópicos</t>
+  </si>
+  <si>
+    <t>Início, Squad</t>
+  </si>
+  <si>
+    <t>2 por semana</t>
+  </si>
+  <si>
+    <r>
+      <t>Feature 08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Funcionalidade Persona 03 – “comex”</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Libras</t>
+    </r>
+  </si>
+  <si>
+    <t>70 - Para motivar o pessoal mais jovem</t>
+  </si>
+  <si>
+    <t>Classificação prioridades</t>
+  </si>
+  <si>
+    <t>F02/F03</t>
+  </si>
+  <si>
+    <t>Sprint Planning Inicial</t>
+  </si>
+  <si>
+    <r>
+      <t>Feature 01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Interface usuários</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Interface parceiros</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Gestão Cupons</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Gestão Vouchers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Módulo de suporte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 06:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Funcionalidade Persona 01 - "tiozaoRH"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 07</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Funcionalidade Persona 02 – “antenada”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Funcionalidade Persona 03 – “comex”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Feature 02 / 03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Interface parceiros e Gestão de Cupons</t>
+    </r>
+  </si>
+  <si>
+    <t>Func. Persona 02 - "Antenada"</t>
+  </si>
+  <si>
+    <t>Points Planejados</t>
+  </si>
+  <si>
+    <t>Points Ajustados</t>
+  </si>
+  <si>
+    <t>Funcionalidades - Valor estimado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2018,8 +2273,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2080,8 +2366,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2184,11 +2494,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2357,6 +2743,122 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="12"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2364,6 +2866,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3484,6 +4029,99 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>8305</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>6357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>750522</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF886C66-E7D4-830B-9E69-98D2F2C45955}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23110093" y="13773645"/>
+          <a:ext cx="742217" cy="357481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>1003790</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>7171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>199782</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>102310</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65A6E589-18AB-DB11-EDF4-CEBF20BA780E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24105578" y="13774459"/>
+          <a:ext cx="733669" cy="461485"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -3788,9 +4426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3820,7 +4456,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
@@ -3858,10 +4494,10 @@
     <row r="9" spans="1:6" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="65" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" s="65" t="s">
         <v>226</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>227</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="8"/>
@@ -3871,7 +4507,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="8"/>
@@ -3881,7 +4517,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="8"/>
@@ -3891,7 +4527,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
@@ -3905,10 +4541,10 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="65" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="8"/>
@@ -3918,7 +4554,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="8"/>
@@ -3928,7 +4564,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="8"/>
@@ -3938,7 +4574,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="8"/>
@@ -3952,10 +4588,10 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="65" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="65" t="s">
         <v>230</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>231</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="8"/>
@@ -3965,7 +4601,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="8"/>
@@ -3975,7 +4611,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="8"/>
@@ -3985,7 +4621,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="8"/>
@@ -3999,10 +4635,10 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="65" t="s">
         <v>233</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>234</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="8"/>
@@ -4012,7 +4648,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="8"/>
@@ -4022,7 +4658,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="8"/>
@@ -4032,7 +4668,7 @@
         <v>11</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="8"/>
@@ -4081,10 +4717,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>236</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
@@ -4092,7 +4728,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="58" x14ac:dyDescent="0.35">
@@ -4100,7 +4736,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="58" x14ac:dyDescent="0.35">
@@ -4108,7 +4744,7 @@
         <v>11</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -4118,10 +4754,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B40" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="58" x14ac:dyDescent="0.35">
@@ -4129,7 +4765,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -4145,7 +4781,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
@@ -4161,7 +4797,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
@@ -4220,249 +4856,249 @@
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B56" s="73" t="s">
+      <c r="B56" s="121" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="73"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73" t="s">
+      <c r="C56" s="121"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="73"/>
-      <c r="G56" s="73"/>
-      <c r="H56" s="73"/>
-      <c r="I56" s="73"/>
-      <c r="J56" s="73"/>
-      <c r="K56" s="73"/>
-      <c r="L56" s="73"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="121"/>
+      <c r="H56" s="121"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="121"/>
+      <c r="K56" s="121"/>
+      <c r="L56" s="121"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B57" s="73"/>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
-      <c r="E57" s="73"/>
-      <c r="F57" s="73"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="73"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="73"/>
-      <c r="K57" s="73"/>
-      <c r="L57" s="73"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="121"/>
+      <c r="D57" s="121"/>
+      <c r="E57" s="121"/>
+      <c r="F57" s="121"/>
+      <c r="G57" s="121"/>
+      <c r="H57" s="121"/>
+      <c r="I57" s="121"/>
+      <c r="J57" s="121"/>
+      <c r="K57" s="121"/>
+      <c r="L57" s="121"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="72"/>
-      <c r="D58" s="72"/>
-      <c r="E58" s="72" t="s">
+      <c r="C58" s="120"/>
+      <c r="D58" s="120"/>
+      <c r="E58" s="120" t="s">
         <v>153</v>
       </c>
-      <c r="F58" s="72"/>
-      <c r="G58" s="72"/>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="72"/>
-      <c r="K58" s="72"/>
-      <c r="L58" s="72"/>
+      <c r="F58" s="120"/>
+      <c r="G58" s="120"/>
+      <c r="H58" s="120"/>
+      <c r="I58" s="120"/>
+      <c r="J58" s="120"/>
+      <c r="K58" s="120"/>
+      <c r="L58" s="120"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
-      <c r="D59" s="72"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="72"/>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="72"/>
-      <c r="L59" s="72"/>
+      <c r="B59" s="120"/>
+      <c r="C59" s="120"/>
+      <c r="D59" s="120"/>
+      <c r="E59" s="120"/>
+      <c r="F59" s="120"/>
+      <c r="G59" s="120"/>
+      <c r="H59" s="120"/>
+      <c r="I59" s="120"/>
+      <c r="J59" s="120"/>
+      <c r="K59" s="120"/>
+      <c r="L59" s="120"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="72"/>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="72"/>
-      <c r="K60" s="72"/>
-      <c r="L60" s="72"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="120"/>
+      <c r="D60" s="120"/>
+      <c r="E60" s="120"/>
+      <c r="F60" s="120"/>
+      <c r="G60" s="120"/>
+      <c r="H60" s="120"/>
+      <c r="I60" s="120"/>
+      <c r="J60" s="120"/>
+      <c r="K60" s="120"/>
+      <c r="L60" s="120"/>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="120" t="s">
         <v>154</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
-      <c r="E61" s="72" t="s">
+      <c r="C61" s="120"/>
+      <c r="D61" s="120"/>
+      <c r="E61" s="120" t="s">
         <v>155</v>
       </c>
-      <c r="F61" s="72"/>
-      <c r="G61" s="72"/>
-      <c r="H61" s="72"/>
-      <c r="I61" s="72"/>
-      <c r="J61" s="72"/>
-      <c r="K61" s="72"/>
-      <c r="L61" s="72"/>
+      <c r="F61" s="120"/>
+      <c r="G61" s="120"/>
+      <c r="H61" s="120"/>
+      <c r="I61" s="120"/>
+      <c r="J61" s="120"/>
+      <c r="K61" s="120"/>
+      <c r="L61" s="120"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B62" s="72"/>
-      <c r="C62" s="72"/>
-      <c r="D62" s="72"/>
-      <c r="E62" s="72"/>
-      <c r="F62" s="72"/>
-      <c r="G62" s="72"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="120"/>
+      <c r="D62" s="120"/>
+      <c r="E62" s="120"/>
+      <c r="F62" s="120"/>
+      <c r="G62" s="120"/>
+      <c r="H62" s="120"/>
+      <c r="I62" s="120"/>
+      <c r="J62" s="120"/>
+      <c r="K62" s="120"/>
+      <c r="L62" s="120"/>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B63" s="72"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="72"/>
-      <c r="H63" s="72"/>
-      <c r="I63" s="72"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="72"/>
-      <c r="L63" s="72"/>
+      <c r="B63" s="120"/>
+      <c r="C63" s="120"/>
+      <c r="D63" s="120"/>
+      <c r="E63" s="120"/>
+      <c r="F63" s="120"/>
+      <c r="G63" s="120"/>
+      <c r="H63" s="120"/>
+      <c r="I63" s="120"/>
+      <c r="J63" s="120"/>
+      <c r="K63" s="120"/>
+      <c r="L63" s="120"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="120" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72" t="s">
+      <c r="C64" s="120"/>
+      <c r="D64" s="120"/>
+      <c r="E64" s="120" t="s">
         <v>157</v>
       </c>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
-      <c r="H64" s="72"/>
-      <c r="I64" s="72"/>
-      <c r="J64" s="72"/>
-      <c r="K64" s="72"/>
-      <c r="L64" s="72"/>
+      <c r="F64" s="120"/>
+      <c r="G64" s="120"/>
+      <c r="H64" s="120"/>
+      <c r="I64" s="120"/>
+      <c r="J64" s="120"/>
+      <c r="K64" s="120"/>
+      <c r="L64" s="120"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="72"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
-      <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="72"/>
-      <c r="L65" s="72"/>
+      <c r="B65" s="120"/>
+      <c r="C65" s="120"/>
+      <c r="D65" s="120"/>
+      <c r="E65" s="120"/>
+      <c r="F65" s="120"/>
+      <c r="G65" s="120"/>
+      <c r="H65" s="120"/>
+      <c r="I65" s="120"/>
+      <c r="J65" s="120"/>
+      <c r="K65" s="120"/>
+      <c r="L65" s="120"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B66" s="72"/>
-      <c r="C66" s="72"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="72"/>
-      <c r="H66" s="72"/>
-      <c r="I66" s="72"/>
-      <c r="J66" s="72"/>
-      <c r="K66" s="72"/>
-      <c r="L66" s="72"/>
+      <c r="B66" s="120"/>
+      <c r="C66" s="120"/>
+      <c r="D66" s="120"/>
+      <c r="E66" s="120"/>
+      <c r="F66" s="120"/>
+      <c r="G66" s="120"/>
+      <c r="H66" s="120"/>
+      <c r="I66" s="120"/>
+      <c r="J66" s="120"/>
+      <c r="K66" s="120"/>
+      <c r="L66" s="120"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="72" t="s">
+      <c r="C67" s="120"/>
+      <c r="D67" s="120"/>
+      <c r="E67" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="F67" s="72"/>
-      <c r="G67" s="72"/>
-      <c r="H67" s="72"/>
-      <c r="I67" s="72"/>
-      <c r="J67" s="72"/>
-      <c r="K67" s="72"/>
-      <c r="L67" s="72"/>
+      <c r="F67" s="120"/>
+      <c r="G67" s="120"/>
+      <c r="H67" s="120"/>
+      <c r="I67" s="120"/>
+      <c r="J67" s="120"/>
+      <c r="K67" s="120"/>
+      <c r="L67" s="120"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B68" s="72"/>
-      <c r="C68" s="72"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="72"/>
-      <c r="H68" s="72"/>
-      <c r="I68" s="72"/>
-      <c r="J68" s="72"/>
-      <c r="K68" s="72"/>
-      <c r="L68" s="72"/>
+      <c r="B68" s="120"/>
+      <c r="C68" s="120"/>
+      <c r="D68" s="120"/>
+      <c r="E68" s="120"/>
+      <c r="F68" s="120"/>
+      <c r="G68" s="120"/>
+      <c r="H68" s="120"/>
+      <c r="I68" s="120"/>
+      <c r="J68" s="120"/>
+      <c r="K68" s="120"/>
+      <c r="L68" s="120"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B69" s="72"/>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="72"/>
-      <c r="G69" s="72"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="72"/>
-      <c r="J69" s="72"/>
-      <c r="K69" s="72"/>
-      <c r="L69" s="72"/>
+      <c r="B69" s="120"/>
+      <c r="C69" s="120"/>
+      <c r="D69" s="120"/>
+      <c r="E69" s="120"/>
+      <c r="F69" s="120"/>
+      <c r="G69" s="120"/>
+      <c r="H69" s="120"/>
+      <c r="I69" s="120"/>
+      <c r="J69" s="120"/>
+      <c r="K69" s="120"/>
+      <c r="L69" s="120"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B70" s="72" t="s">
+      <c r="B70" s="120" t="s">
         <v>160</v>
       </c>
-      <c r="C70" s="72"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72" t="s">
+      <c r="C70" s="120"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="F70" s="72"/>
-      <c r="G70" s="72"/>
-      <c r="H70" s="72"/>
-      <c r="I70" s="72"/>
-      <c r="J70" s="72"/>
-      <c r="K70" s="72"/>
-      <c r="L70" s="72"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="120"/>
+      <c r="H70" s="120"/>
+      <c r="I70" s="120"/>
+      <c r="J70" s="120"/>
+      <c r="K70" s="120"/>
+      <c r="L70" s="120"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B71" s="72"/>
-      <c r="C71" s="72"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="72"/>
-      <c r="F71" s="72"/>
-      <c r="G71" s="72"/>
-      <c r="H71" s="72"/>
-      <c r="I71" s="72"/>
-      <c r="J71" s="72"/>
-      <c r="K71" s="72"/>
-      <c r="L71" s="72"/>
+      <c r="B71" s="120"/>
+      <c r="C71" s="120"/>
+      <c r="D71" s="120"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="120"/>
+      <c r="G71" s="120"/>
+      <c r="H71" s="120"/>
+      <c r="I71" s="120"/>
+      <c r="J71" s="120"/>
+      <c r="K71" s="120"/>
+      <c r="L71" s="120"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B72" s="72"/>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
-      <c r="I72" s="72"/>
-      <c r="J72" s="72"/>
-      <c r="K72" s="72"/>
-      <c r="L72" s="72"/>
+      <c r="B72" s="120"/>
+      <c r="C72" s="120"/>
+      <c r="D72" s="120"/>
+      <c r="E72" s="120"/>
+      <c r="F72" s="120"/>
+      <c r="G72" s="120"/>
+      <c r="H72" s="120"/>
+      <c r="I72" s="120"/>
+      <c r="J72" s="120"/>
+      <c r="K72" s="120"/>
+      <c r="L72" s="120"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B75" s="10"/>
@@ -4548,7 +5184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834B3C7B-1F38-45D0-876C-FF09C5DFDC94}">
   <dimension ref="B3:AE79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" zoomScale="99" zoomScaleNormal="99" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4568,7 +5204,7 @@
   <sheetData>
     <row r="3" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
@@ -4584,7 +5220,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
@@ -4799,7 +5435,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.35">
@@ -4810,7 +5446,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
@@ -4821,7 +5457,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
@@ -4829,7 +5465,7 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="1"/>
       <c r="N28" s="14"/>
@@ -4902,7 +5538,7 @@
     </row>
     <row r="37" spans="2:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="I37" s="40" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
@@ -4924,7 +5560,7 @@
         <v>5</v>
       </c>
       <c r="J39" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K39" s="57">
         <v>1</v>
@@ -4938,10 +5574,10 @@
         <v>8</v>
       </c>
       <c r="J40" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K40" s="60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L40" s="61" t="s">
         <v>202</v>
@@ -4952,7 +5588,7 @@
         <v>21</v>
       </c>
       <c r="J41" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K41" s="57">
         <v>2</v>
@@ -4966,10 +5602,10 @@
         <v>55</v>
       </c>
       <c r="J42" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K42" s="60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L42" s="61" t="s">
         <v>203</v>
@@ -4980,10 +5616,10 @@
         <v>13</v>
       </c>
       <c r="J43" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K43" s="57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L43" s="58" t="s">
         <v>204</v>
@@ -4994,13 +5630,13 @@
         <v>13</v>
       </c>
       <c r="J44" s="43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K44" s="60">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L44" s="61" t="s">
-        <v>206</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
@@ -5008,13 +5644,13 @@
         <v>21</v>
       </c>
       <c r="J45" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K45" s="57">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L45" s="58" t="s">
-        <v>205</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
@@ -5022,10 +5658,10 @@
         <v>34</v>
       </c>
       <c r="J46" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K46" s="60">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L46" s="61" t="s">
         <v>207</v>
@@ -5043,20 +5679,20 @@
         <v>172</v>
       </c>
       <c r="N48" s="40" t="s">
-        <v>209</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="14:19" ht="18.5" x14ac:dyDescent="0.45">
       <c r="N49" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="O49" s="74" t="s">
+      <c r="O49" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="P49" s="74"/>
-      <c r="Q49" s="74"/>
-      <c r="R49" s="74"/>
-      <c r="S49" s="74"/>
+      <c r="P49" s="122"/>
+      <c r="Q49" s="122"/>
+      <c r="R49" s="122"/>
+      <c r="S49" s="122"/>
     </row>
     <row r="50" spans="14:19" x14ac:dyDescent="0.35">
       <c r="N50" s="23" t="s">
@@ -5080,7 +5716,7 @@
     </row>
     <row r="51" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N51" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O51" s="64" t="s">
         <v>169</v>
@@ -5092,7 +5728,7 @@
     </row>
     <row r="52" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N52" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O52" s="60" t="s">
         <v>169</v>
@@ -5104,7 +5740,7 @@
     </row>
     <row r="53" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N53" s="41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="O53" s="64" t="s">
         <v>169</v>
@@ -5116,7 +5752,7 @@
     </row>
     <row r="54" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N54" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O54" s="60"/>
       <c r="P54" s="60" t="s">
@@ -5130,7 +5766,7 @@
     </row>
     <row r="55" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N55" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O55" s="64" t="s">
         <v>169</v>
@@ -5144,7 +5780,7 @@
     </row>
     <row r="56" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N56" s="43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O56" s="60"/>
       <c r="P56" s="60"/>
@@ -5156,7 +5792,7 @@
     </row>
     <row r="57" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N57" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O57" s="64"/>
       <c r="P57" s="64"/>
@@ -5170,7 +5806,7 @@
     </row>
     <row r="58" spans="14:19" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N58" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O58" s="60"/>
       <c r="P58" s="60"/>
@@ -5202,7 +5838,7 @@
         <v>180</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="14:19" x14ac:dyDescent="0.35">
@@ -5210,12 +5846,12 @@
         <v>186</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="30:31" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="AD68" s="40" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="30:31" ht="15.5" x14ac:dyDescent="0.35">
@@ -5228,7 +5864,7 @@
     </row>
     <row r="70" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD70" s="67" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AE70" s="68" t="s">
         <v>201</v>
@@ -5236,7 +5872,7 @@
     </row>
     <row r="71" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD71" s="69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AE71" s="70" t="s">
         <v>202</v>
@@ -5244,7 +5880,7 @@
     </row>
     <row r="72" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD72" s="67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AE72" s="68" t="s">
         <v>203</v>
@@ -5252,7 +5888,7 @@
     </row>
     <row r="73" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD73" s="69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE73" s="70" t="s">
         <v>203</v>
@@ -5260,7 +5896,7 @@
     </row>
     <row r="74" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD74" s="67" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AE74" s="68" t="s">
         <v>204</v>
@@ -5268,7 +5904,7 @@
     </row>
     <row r="75" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD75" s="71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AE75" s="70" t="s">
         <v>206</v>
@@ -5276,7 +5912,7 @@
     </row>
     <row r="76" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD76" s="67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AE76" s="68" t="s">
         <v>205</v>
@@ -5284,7 +5920,7 @@
     </row>
     <row r="77" spans="30:31" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="AD77" s="69" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AE77" s="70" t="s">
         <v>207</v>
@@ -5310,18 +5946,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9C0383-BC9C-4317-9C9B-7E5989B0533C}">
-  <dimension ref="A2:Y75"/>
+  <dimension ref="A2:AG102"/>
   <sheetViews>
-    <sheetView topLeftCell="I44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O58" sqref="O58:V62"/>
+    <sheetView tabSelected="1" topLeftCell="F108" zoomScale="104" zoomScaleNormal="104" workbookViewId="0">
+      <selection activeCell="Q95" sqref="Q95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="43.36328125" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.26953125" customWidth="1"/>
+    <col min="10" max="11" width="9.08984375" customWidth="1"/>
+    <col min="12" max="12" width="44.1796875" customWidth="1"/>
     <col min="13" max="13" width="9.453125" customWidth="1"/>
+    <col min="30" max="30" width="22" customWidth="1"/>
+    <col min="31" max="31" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -5837,7 +6477,13 @@
         <v>166</v>
       </c>
     </row>
+    <row r="43" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="K44" s="79" t="s">
+        <v>284</v>
+      </c>
+      <c r="L44" s="80"/>
+      <c r="M44" s="81"/>
       <c r="O44" t="s">
         <v>181</v>
       </c>
@@ -5849,13 +6495,13 @@
       <c r="J45" t="s">
         <v>191</v>
       </c>
-      <c r="K45" s="27" t="s">
+      <c r="K45" s="82" t="s">
         <v>171</v>
       </c>
       <c r="L45" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="M45" s="23" t="s">
+      <c r="M45" s="83" t="s">
         <v>174</v>
       </c>
     </row>
@@ -5863,13 +6509,13 @@
       <c r="J46" t="s">
         <v>198</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="33">
         <v>5</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="84">
         <v>1</v>
       </c>
       <c r="O46">
@@ -5881,13 +6527,13 @@
       <c r="J47" t="s">
         <v>195</v>
       </c>
-      <c r="K47" s="28">
+      <c r="K47" s="85">
         <v>8</v>
       </c>
       <c r="L47" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="M47" s="24">
+      <c r="M47" s="86">
         <v>2</v>
       </c>
       <c r="O47">
@@ -5899,13 +6545,13 @@
       <c r="J48" t="s">
         <v>196</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="33">
         <v>21</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="84">
         <v>2</v>
       </c>
       <c r="O48">
@@ -5913,76 +6559,76 @@
         <v>336</v>
       </c>
     </row>
-    <row r="49" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:25" x14ac:dyDescent="0.35">
       <c r="J49" t="s">
         <v>193</v>
       </c>
-      <c r="K49" s="28">
+      <c r="K49" s="85">
         <v>55</v>
       </c>
       <c r="L49" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="M49" s="24">
-        <v>4</v>
+      <c r="M49" s="86">
+        <v>3</v>
       </c>
       <c r="O49">
         <f t="shared" si="0"/>
         <v>880</v>
       </c>
     </row>
-    <row r="50" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J50" t="s">
         <v>192</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="35">
         <v>13</v>
       </c>
-      <c r="L50" s="10" t="s">
+      <c r="L50" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="M50">
-        <v>3</v>
+      <c r="M50" s="88">
+        <v>4</v>
       </c>
       <c r="O50">
         <f t="shared" si="0"/>
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:25" x14ac:dyDescent="0.35">
       <c r="J51" t="s">
         <v>198</v>
       </c>
-      <c r="K51" s="28">
-        <v>13</v>
-      </c>
-      <c r="L51" s="29" t="s">
+      <c r="K51" s="89">
+        <v>8</v>
+      </c>
+      <c r="L51" s="90" t="s">
         <v>173</v>
       </c>
-      <c r="M51" s="24">
-        <v>6</v>
+      <c r="M51" s="91">
+        <v>1</v>
       </c>
       <c r="O51">
         <f t="shared" si="0"/>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="52" spans="10:22" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="10:25" x14ac:dyDescent="0.35">
       <c r="J52" t="s">
         <v>197</v>
       </c>
-      <c r="K52" s="1">
-        <v>21</v>
+      <c r="K52" s="33">
+        <v>13</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="M52">
-        <v>7</v>
+      <c r="M52" s="84">
+        <v>1</v>
       </c>
       <c r="O52">
         <f t="shared" ref="O52:O53" si="1">K52*16</f>
-        <v>336</v>
+        <v>208</v>
       </c>
       <c r="Q52">
         <v>8</v>
@@ -5991,22 +6637,22 @@
         <v>183</v>
       </c>
     </row>
-    <row r="53" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J53" t="s">
         <v>194</v>
       </c>
-      <c r="K53" s="28">
-        <v>34</v>
-      </c>
-      <c r="L53" s="24" t="s">
+      <c r="K53" s="92">
+        <v>21</v>
+      </c>
+      <c r="L53" s="93" t="s">
         <v>164</v>
       </c>
-      <c r="M53" s="24">
-        <v>8</v>
+      <c r="M53" s="94">
+        <v>1</v>
       </c>
       <c r="O53">
         <f t="shared" si="1"/>
-        <v>544</v>
+        <v>336</v>
       </c>
       <c r="Q53">
         <v>8</v>
@@ -6015,10 +6661,10 @@
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="10:22" x14ac:dyDescent="0.35">
-      <c r="K54" s="1">
+    <row r="54" spans="10:25" x14ac:dyDescent="0.35">
+      <c r="K54" s="4">
         <f>SUM(K46:K53)</f>
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="L54" s="14"/>
       <c r="Q54">
@@ -6028,13 +6674,13 @@
         <v>185</v>
       </c>
     </row>
-    <row r="55" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:25" x14ac:dyDescent="0.35">
       <c r="K55" s="26" t="s">
         <v>172</v>
       </c>
       <c r="O55">
         <f>SUM(O46:O53)</f>
-        <v>2720</v>
+        <v>2304</v>
       </c>
       <c r="P55">
         <f>8*(20*8)</f>
@@ -6045,56 +6691,64 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="56" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L56" s="13"/>
     </row>
-    <row r="57" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L57" s="14"/>
     </row>
-    <row r="58" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:25" x14ac:dyDescent="0.35">
+      <c r="K58">
+        <f>SUM(K46:K50)</f>
+        <v>102</v>
+      </c>
       <c r="L58" s="14"/>
       <c r="M58" s="24"/>
       <c r="O58" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L59" s="11"/>
       <c r="O59" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L60" s="11"/>
       <c r="O60" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="10:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L61" s="11"/>
       <c r="O61" t="s">
         <v>180</v>
       </c>
       <c r="T61">
-        <v>5</v>
-      </c>
-      <c r="U61" t="s">
+        <v>8</v>
+      </c>
+      <c r="V61" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="62" spans="10:22" x14ac:dyDescent="0.35">
+      <c r="X61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="10:25" x14ac:dyDescent="0.35">
       <c r="L62" s="10"/>
       <c r="O62" t="s">
         <v>186</v>
       </c>
       <c r="T62">
-        <v>40</v>
-      </c>
-      <c r="U62" t="s">
+        <f>T61*8</f>
+        <v>64</v>
+      </c>
+      <c r="V62" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="10:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="10:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="L64" s="13"/>
       <c r="O64" s="1">
         <f>5*8</f>
@@ -6117,12 +6771,15 @@
         <v>40</v>
       </c>
       <c r="T64" s="1"/>
-      <c r="U64" s="25" t="s">
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="V64" s="1"/>
-    </row>
-    <row r="65" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Y64" s="1"/>
+    </row>
+    <row r="65" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K65" s="27" t="s">
         <v>171</v>
       </c>
@@ -6132,39 +6789,47 @@
       <c r="M65" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="O65" s="3" t="s">
+      <c r="N65" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="P65" s="3" t="s">
+      <c r="O65" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="P65" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Q65" s="3" t="s">
+      <c r="Q65" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="R65" s="3" t="s">
+      <c r="R65" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="S65" s="3" t="s">
+      <c r="S65" s="4" t="s">
         <v>176</v>
       </c>
       <c r="T65" s="3"/>
-      <c r="U65" s="30" t="s">
+      <c r="U65" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+      <c r="X65" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="V65" s="31" t="s">
+      <c r="Y65" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="W65" s="31" t="s">
+      <c r="Z65" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="X65" s="31" t="s">
+      <c r="AA65" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="Y65" s="32" t="s">
+      <c r="AB65" s="32" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="11:25" x14ac:dyDescent="0.35">
+    <row r="66" spans="11:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K66" s="1">
         <v>5</v>
       </c>
@@ -6173,6 +6838,9 @@
       </c>
       <c r="M66">
         <v>1</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="O66" s="1">
         <v>5</v>
@@ -6181,24 +6849,39 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="33" t="s">
+      <c r="T66" s="1">
+        <f t="shared" ref="T66:T67" si="3">SUM(O66:S66)</f>
+        <v>5</v>
+      </c>
+      <c r="U66" s="1">
+        <f>K66-T66</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="1" t="str">
+        <f>IF(T66&lt;&gt;K66,"Ajustar","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="W66" s="1"/>
+      <c r="X66" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="V66" s="1"/>
-      <c r="W66" s="1"/>
-      <c r="X66" s="1"/>
-      <c r="Y66" s="34"/>
-    </row>
-    <row r="67" spans="11:25" x14ac:dyDescent="0.35">
-      <c r="K67" s="28">
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="34"/>
+    </row>
+    <row r="67" spans="11:30" x14ac:dyDescent="0.35">
+      <c r="K67" s="73">
         <v>8</v>
       </c>
-      <c r="L67" s="24" t="s">
+      <c r="L67" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="M67" s="24">
+      <c r="M67" s="75">
         <v>2</v>
+      </c>
+      <c r="N67" s="95" t="s">
+        <v>285</v>
       </c>
       <c r="O67" s="1">
         <v>8</v>
@@ -6207,42 +6890,71 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="33" t="s">
+      <c r="T67" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U67" s="1">
+        <f t="shared" ref="U67:U73" si="4">K67-T67</f>
+        <v>0</v>
+      </c>
+      <c r="V67" s="1" t="str">
+        <f t="shared" ref="V67:V73" si="5">IF(T67&lt;&gt;K67,"Ajustar","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="W67" s="1"/>
+      <c r="X67" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="34"/>
-    </row>
-    <row r="68" spans="11:25" x14ac:dyDescent="0.35">
-      <c r="K68" s="1">
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="34"/>
+    </row>
+    <row r="68" spans="11:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K68" s="76">
         <v>21</v>
       </c>
-      <c r="L68" s="10" t="s">
+      <c r="L68" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="M68">
-        <v>2</v>
-      </c>
+      <c r="M68" s="78">
+        <v>3</v>
+      </c>
+      <c r="N68" s="95"/>
       <c r="O68" s="1">
-        <v>21</v>
-      </c>
-      <c r="P68" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="P68" s="1">
+        <v>12</v>
+      </c>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="33" t="s">
+      <c r="T68" s="1">
+        <f>SUM(O68:S68)</f>
+        <v>21</v>
+      </c>
+      <c r="U68" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V68" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W68" s="1"/>
+      <c r="X68" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="34"/>
-    </row>
-    <row r="69" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Y68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z68" s="1"/>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="34"/>
+    </row>
+    <row r="69" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K69" s="28">
         <v>55</v>
       </c>
@@ -6252,28 +6964,40 @@
       <c r="M69" s="24">
         <v>4</v>
       </c>
+      <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="Q69" s="1">
-        <f>55-33</f>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="33"/>
-      <c r="V69" s="1" t="s">
+      <c r="T69" s="1">
+        <f t="shared" ref="T69:T73" si="6">SUM(O69:S69)</f>
+        <v>55</v>
+      </c>
+      <c r="U69" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V69" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W69" s="1"/>
+      <c r="X69" s="33"/>
+      <c r="Y69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="W69" s="1" t="s">
+      <c r="Z69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="34"/>
-    </row>
-    <row r="70" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="34"/>
+    </row>
+    <row r="70" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K70" s="1">
         <v>13</v>
       </c>
@@ -6281,165 +7005,703 @@
         <v>45</v>
       </c>
       <c r="M70">
-        <v>3</v>
-      </c>
-      <c r="O70" s="1">
-        <v>6</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
       <c r="P70" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="33" t="s">
+      <c r="T70" s="1">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="U70" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V70" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W70" s="1"/>
+      <c r="X70" s="33"/>
+      <c r="Y70" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="V70" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="34"/>
-    </row>
-    <row r="71" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="34"/>
+    </row>
+    <row r="71" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K71" s="28">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L71" s="29" t="s">
         <v>173</v>
       </c>
       <c r="M71" s="24">
-        <v>6</v>
-      </c>
-      <c r="O71" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O71" s="1">
+        <v>8</v>
+      </c>
       <c r="P71" s="1"/>
-      <c r="Q71" s="1">
-        <f>K51</f>
-        <v>13</v>
-      </c>
+      <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="33"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1" t="s">
+      <c r="T71" s="1">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="U71" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V71" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W71" s="1"/>
+      <c r="X71" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="34"/>
-    </row>
-    <row r="72" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="34"/>
+    </row>
+    <row r="72" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K72" s="1">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>162</v>
       </c>
       <c r="M72">
-        <v>7</v>
-      </c>
-      <c r="O72" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O72" s="1">
+        <v>13</v>
+      </c>
       <c r="P72" s="1"/>
-      <c r="Q72" s="1">
-        <v>5</v>
-      </c>
-      <c r="R72" s="1">
-        <v>16</v>
-      </c>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
       <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="33"/>
-      <c r="V72" s="1"/>
-      <c r="W72" s="1" t="s">
+      <c r="T72" s="1">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="U72" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V72" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W72" s="1"/>
+      <c r="X72" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="X72" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y72" s="34"/>
-    </row>
-    <row r="73" spans="11:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y72" s="1"/>
+      <c r="Z72" s="1"/>
+      <c r="AA72" s="1"/>
+      <c r="AB72" s="34"/>
+    </row>
+    <row r="73" spans="11:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K73" s="28">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L73" s="24" t="s">
-        <v>164</v>
+        <v>282</v>
       </c>
       <c r="M73" s="24">
-        <v>8</v>
-      </c>
-      <c r="O73" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O73" s="1">
+        <v>21</v>
+      </c>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
-      <c r="R73" s="1">
-        <v>24</v>
-      </c>
-      <c r="S73" s="1">
-        <v>10</v>
-      </c>
-      <c r="T73" s="1"/>
-      <c r="U73" s="35"/>
-      <c r="V73" s="36"/>
-      <c r="W73" s="36"/>
-      <c r="X73" s="36" t="s">
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="U73" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="V73" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>OK</v>
+      </c>
+      <c r="W73" s="1"/>
+      <c r="X73" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="Y73" s="37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Y73" s="36"/>
+      <c r="Z73" s="36"/>
+      <c r="AA73" s="36"/>
+      <c r="AB73" s="37"/>
+    </row>
+    <row r="74" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K74" s="4">
         <f>SUM(K66:K73)</f>
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="L74" s="14"/>
       <c r="O74" s="4">
-        <f>SUM(O66:O73)</f>
-        <v>40</v>
+        <f t="shared" ref="O74:T74" si="7">SUM(O66:O73)</f>
+        <v>64</v>
       </c>
       <c r="P74" s="4">
-        <f>SUM(P66:P73)</f>
-        <v>40</v>
+        <f t="shared" si="7"/>
+        <v>64</v>
       </c>
       <c r="Q74" s="4">
-        <f>SUM(Q66:Q73)</f>
-        <v>40</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
       <c r="R74" s="4">
-        <f>SUM(R66:R73)</f>
-        <v>40</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="S74" s="4">
-        <f>SUM(S66:S73)</f>
-        <v>10</v>
-      </c>
-      <c r="T74" s="4"/>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="T74" s="4">
+        <f t="shared" si="7"/>
+        <v>144</v>
+      </c>
       <c r="U74" s="4"/>
       <c r="V74" s="4"/>
       <c r="W74" s="4"/>
       <c r="X74" s="4"/>
       <c r="Y74" s="4"/>
-    </row>
-    <row r="75" spans="11:25" x14ac:dyDescent="0.35">
+      <c r="Z74" s="4"/>
+      <c r="AA74" s="4"/>
+      <c r="AB74" s="4"/>
+    </row>
+    <row r="75" spans="11:30" x14ac:dyDescent="0.35">
       <c r="K75" s="26" t="s">
         <v>172</v>
       </c>
     </row>
+    <row r="78" spans="11:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K78" s="96"/>
+      <c r="L78" s="96"/>
+      <c r="M78" s="96"/>
+      <c r="N78" s="96"/>
+    </row>
+    <row r="79" spans="11:30" x14ac:dyDescent="0.35">
+      <c r="K79" s="96"/>
+      <c r="L79" s="97" t="s">
+        <v>126</v>
+      </c>
+      <c r="M79" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="N79" s="96"/>
+      <c r="AD79" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="80" spans="11:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K80" s="96"/>
+      <c r="L80" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="M80" s="100">
+        <v>1</v>
+      </c>
+      <c r="N80" s="96"/>
+      <c r="AD80" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="81" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K81" s="96"/>
+      <c r="L81" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="M81" s="75">
+        <v>2</v>
+      </c>
+      <c r="N81" s="96"/>
+    </row>
+    <row r="82" spans="9:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K82" s="96"/>
+      <c r="L82" s="102" t="s">
+        <v>41</v>
+      </c>
+      <c r="M82" s="78">
+        <v>3</v>
+      </c>
+      <c r="N82" s="96"/>
+      <c r="AF82" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="AG82" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="83" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K83" s="96"/>
+      <c r="L83" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="M83" s="86">
+        <v>4</v>
+      </c>
+      <c r="N83" s="96"/>
+      <c r="R83" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD83" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE83" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF83" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG83" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="84" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K84" s="96"/>
+      <c r="L84" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="M84" s="100">
+        <v>5</v>
+      </c>
+      <c r="N84" s="96"/>
+      <c r="AD84" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE84" t="s">
+        <v>277</v>
+      </c>
+      <c r="AG84" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="85" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K85" s="96"/>
+      <c r="L85" s="104" t="s">
+        <v>173</v>
+      </c>
+      <c r="M85" s="86">
+        <v>1</v>
+      </c>
+      <c r="N85" s="96"/>
+      <c r="AD85" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE85" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF85" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="86" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K86" s="96"/>
+      <c r="L86" s="99" t="s">
+        <v>162</v>
+      </c>
+      <c r="M86" s="100">
+        <v>1</v>
+      </c>
+      <c r="N86" s="96"/>
+      <c r="R86" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD86" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE86" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF86" t="s">
+        <v>268</v>
+      </c>
+      <c r="AG86" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="9:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K87" s="96"/>
+      <c r="L87" s="105" t="s">
+        <v>282</v>
+      </c>
+      <c r="M87" s="94">
+        <v>1</v>
+      </c>
+      <c r="N87" s="96"/>
+      <c r="R87" t="s">
+        <v>272</v>
+      </c>
+      <c r="AD87" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE87" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF87" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG87" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="88" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="K88" s="96"/>
+      <c r="L88" s="96"/>
+      <c r="M88" s="96"/>
+      <c r="N88" s="96"/>
+      <c r="AD88" t="s">
+        <v>265</v>
+      </c>
+      <c r="AE88" t="s">
+        <v>278</v>
+      </c>
+      <c r="AF88" t="s">
+        <v>280</v>
+      </c>
+      <c r="AG88" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="89" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="AD89" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE89" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF89" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG89" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="93" spans="9:33" x14ac:dyDescent="0.35">
+      <c r="I93" s="96"/>
+    </row>
+    <row r="94" spans="9:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I94" s="96"/>
+      <c r="J94" s="96"/>
+      <c r="K94" s="96"/>
+      <c r="L94" s="96"/>
+      <c r="M94" s="96"/>
+      <c r="N94" s="96"/>
+      <c r="O94" s="96"/>
+    </row>
+    <row r="95" spans="9:33" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I95" s="96"/>
+      <c r="J95" s="129" t="s">
+        <v>297</v>
+      </c>
+      <c r="K95" s="129" t="s">
+        <v>298</v>
+      </c>
+      <c r="L95" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="M95" s="114" t="s">
+        <v>174</v>
+      </c>
+      <c r="N95" s="115" t="s">
+        <v>106</v>
+      </c>
+      <c r="O95" s="96"/>
+    </row>
+    <row r="96" spans="9:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I96" s="96"/>
+      <c r="J96" s="130">
+        <v>5</v>
+      </c>
+      <c r="K96" s="130">
+        <v>5</v>
+      </c>
+      <c r="L96" s="125" t="s">
+        <v>31</v>
+      </c>
+      <c r="M96" s="126">
+        <v>1</v>
+      </c>
+      <c r="N96" s="116" t="s">
+        <v>131</v>
+      </c>
+      <c r="O96" s="96"/>
+    </row>
+    <row r="97" spans="9:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I97" s="96"/>
+      <c r="J97" s="134">
+        <v>29</v>
+      </c>
+      <c r="K97" s="134">
+        <v>25</v>
+      </c>
+      <c r="L97" s="135" t="s">
+        <v>295</v>
+      </c>
+      <c r="M97" s="135">
+        <v>2</v>
+      </c>
+      <c r="N97" s="136" t="s">
+        <v>285</v>
+      </c>
+      <c r="O97" s="96"/>
+    </row>
+    <row r="98" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="I98" s="96"/>
+      <c r="J98" s="131">
+        <v>8</v>
+      </c>
+      <c r="K98" s="131">
+        <v>6</v>
+      </c>
+      <c r="L98" s="127" t="s">
+        <v>173</v>
+      </c>
+      <c r="M98" s="128">
+        <v>1</v>
+      </c>
+      <c r="N98" s="137" t="s">
+        <v>136</v>
+      </c>
+      <c r="O98" s="96"/>
+    </row>
+    <row r="99" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="I99" s="96"/>
+      <c r="J99" s="130">
+        <v>13</v>
+      </c>
+      <c r="K99" s="130">
+        <v>10</v>
+      </c>
+      <c r="L99" s="125" t="s">
+        <v>162</v>
+      </c>
+      <c r="M99" s="126">
+        <v>1</v>
+      </c>
+      <c r="N99" s="116" t="s">
+        <v>137</v>
+      </c>
+      <c r="O99" s="96"/>
+    </row>
+    <row r="100" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="I100" s="96"/>
+      <c r="J100" s="131">
+        <v>21</v>
+      </c>
+      <c r="K100" s="131">
+        <v>18</v>
+      </c>
+      <c r="L100" s="128" t="s">
+        <v>282</v>
+      </c>
+      <c r="M100" s="128">
+        <v>1</v>
+      </c>
+      <c r="N100" s="137" t="s">
+        <v>138</v>
+      </c>
+      <c r="O100" s="96"/>
+    </row>
+    <row r="101" spans="9:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I101" s="96"/>
+      <c r="J101" s="133">
+        <f>SUM(J96:J100)</f>
+        <v>76</v>
+      </c>
+      <c r="K101" s="132">
+        <f>SUM(K96:K100)</f>
+        <v>64</v>
+      </c>
+      <c r="L101" s="117"/>
+      <c r="M101" s="118"/>
+      <c r="N101" s="119"/>
+      <c r="O101" s="96"/>
+    </row>
+    <row r="102" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="I102" s="96"/>
+      <c r="J102" s="96"/>
+      <c r="K102" s="96"/>
+      <c r="L102" s="96"/>
+      <c r="M102" s="96"/>
+      <c r="N102" s="96"/>
+      <c r="O102" s="96"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A447F868-EEBF-438E-B55C-11694AE044F9}">
+  <dimension ref="A2:D13"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="47.36328125" customWidth="1"/>
+    <col min="3" max="3" width="56.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+    </row>
+    <row r="3" spans="1:4" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="96"/>
+      <c r="B3" s="123" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="124"/>
+      <c r="D3" s="96"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="96"/>
+      <c r="B4" s="106" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="107" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" s="96"/>
+    </row>
+    <row r="5" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="96"/>
+      <c r="B5" s="108" t="s">
+        <v>287</v>
+      </c>
+      <c r="C5" s="109" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="96"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="96"/>
+      <c r="B6" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="111" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="96"/>
+    </row>
+    <row r="7" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="96"/>
+      <c r="B7" s="108" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="109" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="96"/>
+    </row>
+    <row r="8" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="96"/>
+      <c r="B8" s="110" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="96"/>
+    </row>
+    <row r="9" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="96"/>
+      <c r="B9" s="108" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="109" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="96"/>
+    </row>
+    <row r="10" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="96"/>
+      <c r="B10" s="110" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="111" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="96"/>
+    </row>
+    <row r="11" spans="1:4" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="96"/>
+      <c r="B11" s="108" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="96"/>
+    </row>
+    <row r="12" spans="1:4" ht="27.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="96"/>
+      <c r="B12" s="112" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" s="113" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="96"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="96"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C92B289-1327-43A2-9FC5-B021202794DA}">
   <dimension ref="A3:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -6974,7 +8236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5052A683-FA1C-4DA9-9E26-20B7BD0EC11B}">
   <dimension ref="B3:E19"/>
   <sheetViews>

</xml_diff>